<commit_message>
Added experimental design for one of the questions
</commit_message>
<xml_diff>
--- a/Inferential Statistics- Final Project(Udacity).xlsx
+++ b/Inferential Statistics- Final Project(Udacity).xlsx
@@ -6,6 +6,10 @@
     <sheet state="visible" name="Introduction" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="Dataset" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Research Question &amp; Hypothesis" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="ExperimentalDesignResearch Ques" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="ResultsResearch Question &amp; Hypo" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="Sheet12" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="Sheet13" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,48 +17,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t>Specific Question</t>
+  </si>
+  <si>
+    <t>Possible Lurking Variables</t>
+  </si>
+  <si>
+    <t>Hypothesis</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Age of patient at time of operation</t>
+  </si>
+  <si>
     <t>Introduction and Description:</t>
   </si>
   <si>
-    <t>Age of patient at time of operation</t>
-  </si>
-  <si>
-    <t>Specific Question</t>
-  </si>
-  <si>
-    <t>Possible Lurking Variables</t>
-  </si>
-  <si>
-    <t>Hypothesis</t>
-  </si>
-  <si>
-    <t>Releationship between age of patient at the time of operation and number of positive axillary nodes detected</t>
-  </si>
-  <si>
-    <t>Can we say that a specific age group have chances of getting higher/lower number of positive axillary nodes detected? Is there any trend?</t>
-  </si>
-  <si>
-    <t>Think in detail later.</t>
-  </si>
-  <si>
-    <t>H0: There is no relationship between age group and the number of postive axillary nodes detected.</t>
-  </si>
-  <si>
     <t>Importance of analyzing and understanding the results:</t>
   </si>
   <si>
     <t>Things to know:</t>
-  </si>
-  <si>
-    <t>Patient's year of operation</t>
-  </si>
-  <si>
-    <t>Number of positive axillary nodes detected</t>
   </si>
   <si>
     <t>The dataset contains cases from a study that was conducted between
@@ -63,6 +52,12 @@
    cancer.</t>
   </si>
   <si>
+    <t>Patient's year of operation</t>
+  </si>
+  <si>
+    <t>Number of positive axillary nodes detected</t>
+  </si>
+  <si>
     <t>Survival status</t>
   </si>
   <si>
@@ -70,9 +65,6 @@
   </si>
   <si>
     <t>Positive axillary nodes: A positive axillary lymph node is a lymph node in the area of the armpit (axilla) to which cancer has spread.</t>
-  </si>
-  <si>
-    <t>Relationship between age of patient at the time of operation and survival status post operation</t>
   </si>
   <si>
     <t>Number of Instances: 306</t>
@@ -114,35 +106,176 @@
     <t>Many questions like above can be answered by analyzing the given dataset, which can be very helpful to understand the behaviour and pattern between the disease and the concerned patients. Having these answers the doctors/government can proceed in a way to tackle the situation more effectively.</t>
   </si>
   <si>
+    <t>Pattern of age of pateint at the time of operation, to see the trend on which age the disease often affects</t>
+  </si>
+  <si>
+    <t>What are the descriptive statistics for the age of pateints at the time of operation?</t>
+  </si>
+  <si>
+    <t>There might be lesser number of samples for higher age.</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pattern of year of treatment, to see the trend</t>
+  </si>
+  <si>
+    <t>What are the descriptive statistics for the patients year of operation?</t>
+  </si>
+  <si>
+    <t>Pattern of number of positive axillary detected at the time of operation, to see the trend</t>
+  </si>
+  <si>
+    <t>What are the descriptive statistics for the number of positive axillary nodes detected?</t>
+  </si>
+  <si>
+    <t>Releationship between age of patient at the time of operation and number of positive axillary nodes detected</t>
+  </si>
+  <si>
+    <t>Can we say that a specific age group have chances of getting higher/lower number of positive axillary nodes detected? Is there any trend?</t>
+  </si>
+  <si>
+    <t>There might be lesser number of samples for higher age group as few people only live that long.</t>
+  </si>
+  <si>
+    <t>H0: Both the age groups (30-47 and 48-65) will have around same number of positive axillary nodes detected.
+UA=UB
+HA: The groups will have significantly different number of postive axillary nodes detected.
+UA&lt;&gt;UB</t>
+  </si>
+  <si>
+    <t>I support the alternative hypothesis here.</t>
+  </si>
+  <si>
+    <t>Relationship between age of patient at the time of operation and survival status post operation</t>
+  </si>
+  <si>
+    <t>Can we say that the treatment affects different age groups differently?</t>
+  </si>
+  <si>
     <t>Change in survival status of patients with the year in which operation is performed</t>
   </si>
   <si>
+    <t>Can we say that the treatment has become better/worse with time in delivering positive results?</t>
+  </si>
+  <si>
     <t>Relationship between number of positive axillary nodes detected and survival status</t>
   </si>
   <si>
-    <t>Relationship between age of patient at the time of operation and year of operation, to know if the patients are becoming more aware to get diagonsed at an earlier stage with time or may be to see if with time the disease is changing the age group to attack upon, if yes which direction</t>
-  </si>
-  <si>
-    <t>Change in number of postive axillary nodes detected with the year in which operation is performed, to know if the disease is becoming more or less severe with time.</t>
-  </si>
-  <si>
-    <t>Pattern of age of pateint at the time of operation, to see the trend on which age the disease often affects</t>
-  </si>
-  <si>
-    <t>Pattern of year of treatment, to see the trend</t>
-  </si>
-  <si>
-    <t>Pattern of number of positive axillary detected at the time of operation, to see the trend</t>
-  </si>
-  <si>
-    <t>Question 2, 3 and 4 can be clubbed to work as multiple regression, to create a single equation</t>
+    <t>Is there any relationship between number of positive axillary nodes detected and survival rate?</t>
+  </si>
+  <si>
+    <t>Relationship between age of patient at the time of operation and year of operation, to know if the patients are becoming more aware to get diagonsed at an earlier stage with time or may be to see if with time the disease is changing the age group to attack upon, if yes which direction. The latter question makes more sense here.</t>
+  </si>
+  <si>
+    <t>Is there change in the affected age group with time?</t>
+  </si>
+  <si>
+    <t>Change in number of positive axillary nodes detected with the year in which operation is performed, to know if the disease is becoming more or less severe with time. Or if we are becoming more able to detect the positive axillary nodes with time. The latter one is quite an unlikely question though.</t>
+  </si>
+  <si>
+    <t>Is the disease becmoning more severe with time?</t>
+  </si>
+  <si>
+    <t>Question 7, 8 and 9 have to be done with CHI^2 test becuase the attribute status is of nominal type.</t>
+  </si>
+  <si>
+    <t>All questions having time(year of operation) as variable can be made to undergone ANOVA or t tests in longitudinal category</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>The above data gives descriptive statistics about the age of patients being diagonsed with Breast Cancer.</t>
+  </si>
+  <si>
+    <t>The distribution is very normal and have central tendency as 52. So we can say the average age of a person undergoing a breast cancer operation is 52 years.
+Thus, it can be indirectly inferred that the age group 41-63 is most prone to breast cancer.</t>
+  </si>
+  <si>
+    <t>The above data gives descriptive statistics about the year of patients being diagonsed with Breast Cancer.</t>
+  </si>
+  <si>
+    <t>There is around 3 times decrease in the count in the year 1968 as compared to that of 1958.
+Also the distribution is quite skewed and its very difficult to deduce any specific information from it.</t>
+  </si>
+  <si>
+    <t>30-47</t>
+  </si>
+  <si>
+    <t>48-65</t>
+  </si>
+  <si>
+    <t>66-83</t>
+  </si>
+  <si>
+    <t>Can we say that a specific age group have chances of getting higher/lower number of positive axillary nodes detected?
+Is there any trend?</t>
+  </si>
+  <si>
+    <t>The above data gives descriptive statistics about the number of positive axillary nodes detetcted for pateints with Breast Cancer being diagonsed.</t>
+  </si>
+  <si>
+    <t>The distribution is highly positively skewed having mean, median and mode all fell at extreme left end.
+This means, in general pateints having Breast Cancer being diagoned have around 0 to 4 number of positive axillary nodes.</t>
+  </si>
+  <si>
+    <t>Above we can see the graph between age of patients and the number of positive axillary nodes detected during treatment.
+We have divided the given data into three age groups in the left namely 30 to 47, 48 to 65 and 66 to 83.
+We want to know if any of these groups have significantly different number of positive axillary nodes found than any other group.</t>
+  </si>
+  <si>
+    <t>Let us see how the graphs looks like for all the three age groups we have created:</t>
+  </si>
+  <si>
+    <t>Let's see if the given data satisfies the assumptions for One-Way ANOVA:</t>
+  </si>
+  <si>
+    <t>* First of all, let us check the normality of the age groups:</t>
+  </si>
+  <si>
+    <t>Ranges from 0 to 52, with most values at the low end. The median is 1.</t>
+  </si>
+  <si>
+    <t>Ranges from 0 to 46, with most values at the low end. The median is 1.</t>
+  </si>
+  <si>
+    <t>Ranges from 0 to 14.</t>
+  </si>
+  <si>
+    <t>As clear from the above distributions that the samples are quite assymetrical, but still we can ignore the normality asumption as the size of the samples are quite large in each of the above case. (n&gt;30)</t>
+  </si>
+  <si>
+    <t>* Let us move to check the homogeneity of variances:</t>
+  </si>
+  <si>
+    <t>The variance of the third group is quite different. Moreover, we can't ignore this as the sample sizes of all the groups are significantly different.</t>
+  </si>
+  <si>
+    <t>This means these groups of data are not suitable for running ANOVA.</t>
+  </si>
+  <si>
+    <t>Let's just consider the first two groups. As the variance is also not significanlty different between these two groups, these becomes a good subject for t-test.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -152,13 +285,28 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF616161"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF616161"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -172,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -188,12 +336,424 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Number of positive axillary nodes detected vs. Age of patient at time of operation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dataset!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="3366CC"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Dataset!$A$2:$A$307</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Dataset!$C$2:$C$307</c:f>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1884226058"/>
+        <c:axId val="1973772077"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1884226058"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="83.0"/>
+          <c:min val="30.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="757575"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Age of patient at time of operation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1973772077"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1973772077"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="52.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr i="0" sz="1200">
+                    <a:solidFill>
+                      <a:srgbClr val="757575"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Number of positive axillary nodes detected</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1884226058"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>30-47, 48-65 and 66-83</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ExperimentalDesignResearch Ques'!$A$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ExperimentalDesignResearch Ques'!$A$2:$A$162</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ExperimentalDesignResearch Ques'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ExperimentalDesignResearch Ques'!$B$2:$B$162</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ExperimentalDesignResearch Ques'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ExperimentalDesignResearch Ques'!$C$2:$C$162</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="896613646"/>
+        <c:axId val="1102335311"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="896613646"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1102335311"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1102335311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="52.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896613646"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+  </c:chart>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -205,6 +765,83 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -222,67 +859,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -308,16 +945,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -333,6 +970,7 @@
       <c r="D2" s="3">
         <v>1.0</v>
       </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="3">
@@ -347,6 +985,7 @@
       <c r="D3" s="3">
         <v>1.0</v>
       </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="3">
@@ -361,6 +1000,7 @@
       <c r="D4" s="3">
         <v>1.0</v>
       </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="3">
@@ -375,6 +1015,7 @@
       <c r="D5" s="3">
         <v>1.0</v>
       </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="3">
@@ -389,6 +1030,7 @@
       <c r="D6" s="3">
         <v>1.0</v>
       </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="3">
@@ -403,6 +1045,7 @@
       <c r="D7" s="3">
         <v>1.0</v>
       </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="3">
@@ -4616,10 +5259,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="45.57"/>
-    <col customWidth="1" min="2" max="2" width="48.29"/>
-    <col customWidth="1" min="3" max="3" width="48.0"/>
-    <col customWidth="1" min="4" max="4" width="46.14"/>
+    <col customWidth="1" min="1" max="1" width="37.57"/>
+    <col customWidth="1" min="2" max="2" width="39.43"/>
+    <col customWidth="1" min="3" max="3" width="38.71"/>
+    <col customWidth="1" min="4" max="4" width="35.57"/>
+    <col customWidth="1" min="5" max="5" width="34.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4627,94 +5271,1770 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B19" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B22" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3">
+        <v>21.0</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B29" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B31" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B32" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B33" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B37" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C37" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B38" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B39" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B40" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B42" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B44" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3">
+        <v>23.0</v>
+      </c>
+      <c r="B45" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B51" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B53" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B54" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B55" s="3">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B56" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57">
+        <f>AVERAGE(A2:A162)</f>
+        <v>4.38317757</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H57">
+        <f>AVERAGE(B2:B162)</f>
+        <v>4.291925466</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L57">
+        <f>AVERAGE(C2:C162)</f>
+        <v>1.894736842</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58">
+        <f>MEDIAN(A1:A162)</f>
+        <v>1</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H58">
+        <f>MEDIAN(B1:B162)</f>
+        <v>1</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L58">
+        <f>MEDIAN(C1:C162)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B59" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59">
+        <f>MODE(A1:A162)</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H59">
+        <f>MODE(B1:B162)</f>
+        <v>0</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L59">
+        <f>MODE(C1:C162)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60">
+        <f>STDEV(A1:A162)</f>
+        <v>7.797731721</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H60">
+        <f>STDEV(B1:B162)</f>
+        <v>7.351564248</v>
+      </c>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L60">
+        <f>STDEV(C1:C162)</f>
+        <v>3.585175737</v>
+      </c>
+      <c r="M60" s="7"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B62" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B63" s="3">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3">
+        <v>52.0</v>
+      </c>
+      <c r="B64" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B65" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B66" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B67" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="B68" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B69" s="3">
+        <v>46.0</v>
+      </c>
+      <c r="E69" s="9"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B70" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B71" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B72" s="3">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B74" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B75" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="B76" s="3">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3">
+        <v>19.0</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B78" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B80" s="3">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3">
+        <v>16.0</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B82" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B83" s="3">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B85" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B86" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="B87" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B88" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B90" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B91" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B92" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="B93" s="3">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B95" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B96" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B97" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3">
+        <v>23.0</v>
+      </c>
+      <c r="B98" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B99" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B100" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B101" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B102" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B103" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B104" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B105" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B106" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B107" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="B108" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" s="3">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" s="3">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" s="3">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" s="3">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" s="3">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" s="3">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="B142" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146" s="3">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147" s="3">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="B148" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" s="3">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="B151" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="B152" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="B153" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="B154" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="B155" s="3">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="B156" s="3">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="B157" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="B158" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="B159" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="B160" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="B161" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E45:J45"/>
+    <mergeCell ref="E46:J46"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="E67:J67"/>
+    <mergeCell ref="E64:J64"/>
+    <mergeCell ref="E65:J65"/>
+    <mergeCell ref="E68:J68"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="E62:J62"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="8" max="8" width="21.14"/>
+    <col customWidth="1" min="9" max="9" width="21.71"/>
+    <col customWidth="1" min="10" max="10" width="21.0"/>
+    <col customWidth="1" min="11" max="11" width="20.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="H3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="H4">
+        <v>52.45751633986928</v>
+      </c>
+      <c r="I4">
+        <v>52.0</v>
+      </c>
+      <c r="J4">
+        <v>52.0</v>
+      </c>
+      <c r="K4">
+        <v>10.803452349303296</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="H6" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="H8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H8:K8"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="8" max="8" width="21.57"/>
+    <col customWidth="1" min="9" max="9" width="20.71"/>
+    <col customWidth="1" min="10" max="10" width="20.43"/>
+    <col customWidth="1" min="11" max="11" width="21.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="H3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="H4">
+        <v>62.85294117647059</v>
+      </c>
+      <c r="I4">
+        <v>63.0</v>
+      </c>
+      <c r="J4">
+        <v>58.0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3.249404663</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="H6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="H8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H8:K8"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="8" max="8" width="21.14"/>
+    <col customWidth="1" min="9" max="9" width="21.0"/>
+    <col customWidth="1" min="10" max="10" width="20.57"/>
+    <col customWidth="1" min="11" max="11" width="20.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="H3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="H4">
+        <v>4.026143790849673</v>
+      </c>
+      <c r="I4">
+        <v>1.0</v>
+      </c>
+      <c r="J4">
+        <v>0.0</v>
+      </c>
+      <c r="K4">
+        <v>7.189653506248556</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="H6" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="H8" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H8:K8"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>